<commit_message>
update report audit log
</commit_message>
<xml_diff>
--- a/data/reporting/Audit_Log_Report.xlsx
+++ b/data/reporting/Audit_Log_Report.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="720" yWindow="465" windowWidth="17955" windowHeight="11985"/>
   </bookViews>
   <sheets>
-    <sheet name="COURSE REPORT" sheetId="1" r:id="rId1"/>
+    <sheet name="AUDIT LOG REPORT" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -429,7 +429,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix remaining issues in phase 1b
</commit_message>
<xml_diff>
--- a/data/reporting/Audit_Log_Report.xlsx
+++ b/data/reporting/Audit_Log_Report.xlsx
@@ -19,37 +19,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Time Stamp</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Data field</t>
+  </si>
+  <si>
+    <t>Previous value</t>
+  </si>
+  <si>
+    <t>New value</t>
+  </si>
+  <si>
+    <t>Table name</t>
+  </si>
+  <si>
     <t>NTID</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Time Stamp</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Data field</t>
-  </si>
-  <si>
-    <t>Previous value</t>
-  </si>
-  <si>
-    <t>New value</t>
-  </si>
-  <si>
-    <t>Table name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -125,11 +128,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,46 +444,46 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
     <col min="3" max="7" width="26.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="58.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="37.85546875" style="11" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>2</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -495,57 +501,57 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -558,7 +564,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="9"/>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -568,7 +574,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>

</xml_diff>